<commit_message>
edited search_workflow and ballpoint pen example
</commit_message>
<xml_diff>
--- a/examples/Data_inputs_ballpoint_pen_example.xlsx
+++ b/examples/Data_inputs_ballpoint_pen_example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ek2517/Documents/GitHub/ARIA/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49369A20-0761-E14F-997F-B423FEE0B663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40316566-347E-FC4E-9135-DE5F1EA93C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33300" yWindow="2420" windowWidth="30240" windowHeight="17700" xr2:uid="{3367ADF2-404E-8249-84D1-C6000992A6DA}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17700" xr2:uid="{3367ADF2-404E-8249-84D1-C6000992A6DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>